<commit_message>
Update Something in Gen_gcode
</commit_message>
<xml_diff>
--- a/excel/time_processing.xlsx
+++ b/excel/time_processing.xlsx
@@ -162,7 +162,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -212,7 +212,7 @@
       <row>2</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -262,7 +262,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -312,7 +312,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -362,7 +362,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="10" name="Image 10" descr="Picture"/>
@@ -412,7 +412,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="12" name="Image 12" descr="Picture"/>
@@ -462,7 +462,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="14" name="Image 14" descr="Picture"/>
@@ -512,7 +512,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="16" name="Image 16" descr="Picture"/>
@@ -562,7 +562,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="18" name="Image 18" descr="Picture"/>
@@ -612,7 +612,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="20" name="Image 20" descr="Picture"/>
@@ -637,7 +637,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="695325" cy="952500"/>
+    <ext cx="638175" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="21" name="Image 21" descr="Picture"/>
@@ -662,7 +662,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="22" name="Image 22" descr="Picture"/>
@@ -712,7 +712,7 @@
       <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="24" name="Image 24" descr="Picture"/>
@@ -762,7 +762,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="26" name="Image 26" descr="Picture"/>
@@ -787,7 +787,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="638175" cy="952500"/>
+    <ext cx="533400" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="27" name="Image 27" descr="Picture"/>
@@ -812,7 +812,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="28" name="Image 28" descr="Picture"/>
@@ -837,7 +837,7 @@
       <row>15</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="714375" cy="952500"/>
+    <ext cx="533400" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="29" name="Image 29" descr="Picture"/>
@@ -862,7 +862,7 @@
       <row>15</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="676275" cy="952500"/>
+    <ext cx="952500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="30" name="Image 30" descr="Picture"/>
@@ -1222,11 +1222,11 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.391</v>
+        <v>1.373</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>922</v>
+        <v>575</v>
       </c>
     </row>
     <row r="3" ht="85" customHeight="1">
@@ -1237,11 +1237,11 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>2.108</v>
+        <v>1.251</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>1131</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" ht="85" customHeight="1">
@@ -1252,11 +1252,11 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>1.929</v>
+        <v>1.28</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>1022</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" ht="85" customHeight="1">
@@ -1267,11 +1267,11 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>1.428</v>
+        <v>1.323</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>782</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" ht="85" customHeight="1">
@@ -1282,11 +1282,11 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>1.403</v>
+        <v>1.291</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>1297</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" ht="85" customHeight="1">
@@ -1297,11 +1297,11 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>1.37</v>
+        <v>1.274</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>1366</v>
+        <v>910</v>
       </c>
     </row>
     <row r="8" ht="85" customHeight="1">
@@ -1312,11 +1312,11 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>1.338</v>
+        <v>1.215</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>1195</v>
+        <v>707</v>
       </c>
     </row>
     <row r="9" ht="85" customHeight="1">
@@ -1327,11 +1327,11 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>1.35</v>
+        <v>1.349</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>1583</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="10" ht="85" customHeight="1">
@@ -1342,11 +1342,11 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>1.296</v>
+        <v>1.216</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>1078</v>
+        <v>819</v>
       </c>
     </row>
     <row r="11" ht="85" customHeight="1">
@@ -1357,11 +1357,11 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>1.324</v>
+        <v>1.171</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>1200</v>
+        <v>752</v>
       </c>
     </row>
     <row r="12" ht="85" customHeight="1">
@@ -1372,11 +1372,11 @@
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
-        <v>1.349</v>
+        <v>1.125</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>2077</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" ht="85" customHeight="1">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>2.531</v>
+        <v>1.198</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>1089</v>
+        <v>581</v>
       </c>
     </row>
     <row r="14" ht="85" customHeight="1">
@@ -1402,11 +1402,11 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.555</v>
+        <v>1.205</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>1359</v>
+        <v>656</v>
       </c>
     </row>
     <row r="15" ht="85" customHeight="1">
@@ -1417,11 +1417,11 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
-        <v>1.41</v>
+        <v>1.268</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>1700</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="16" ht="85" customHeight="1">
@@ -1432,11 +1432,11 @@
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
-        <v>1.3</v>
+        <v>1.259</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>1049</v>
+        <v>598</v>
       </c>
     </row>
     <row r="17">
@@ -1444,7 +1444,7 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 23.082 giây</t>
+          <t>TỔNG: 18.798 giây</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>

</xml_diff>